<commit_message>
commit na avond op 27/11
</commit_message>
<xml_diff>
--- a/res/test.xlsx
+++ b/res/test.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="29">
   <si>
     <t>MeerkeuzeVraag</t>
   </si>
@@ -59,7 +59,7 @@
     <t>UML patronen aanduiden</t>
   </si>
   <si>
-    <t>Titatovenaar</t>
+    <t>In een bestaande UML moet je alle gebruikte patronen kunnen herkennen, benoemen en aanduiden.</t>
   </si>
   <si>
     <t>Java heeft geen ondersteuning voor het Observer pattern</t>
@@ -80,7 +80,7 @@
     <t>Ontwerp patronen</t>
   </si>
   <si>
-    <t>YOLO</t>
+    <t>De definitie van een ontwerp patroon moet je kunnen herkennen</t>
   </si>
   <si>
     <t>Welk ontwerp principe is het minst van toepassing op het Strategy patroon?</t>
@@ -99,9 +99,6 @@
   </si>
   <si>
     <t>Converteert één interface naar een andere</t>
-  </si>
-  <si>
-    <t>De definitie van een ontwerp patroon moet je kunnen herkennen</t>
   </si>
 </sst>
 </file>
@@ -152,55 +149,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-    </row>
+    <row r="1"/>
+    <row r="2"/>
     <row r="3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E3" t="s">
         <v>3</v>
@@ -209,7 +171,7 @@
         <v>4</v>
       </c>
       <c r="G3" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H3" t="s">
         <v>6</v>
@@ -228,30 +190,39 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="E5" t="s">
-        <v>13</v>
+        <v>3</v>
+      </c>
+      <c r="F5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H5" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="6">
       <c r="B6" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C6" t="n">
         <v>1.0</v>
       </c>
       <c r="D6" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7">
@@ -259,75 +230,66 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E7" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" t="s">
         <v>19</v>
       </c>
-      <c r="C8" t="n">
+      <c r="C10" t="n">
         <v>2.0</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D10" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="B9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="D9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" t="s">
-        <v>5</v>
-      </c>
-      <c r="E10" t="s">
-        <v>3</v>
-      </c>
-      <c r="F10" t="s">
-        <v>4</v>
-      </c>
-      <c r="G10" t="s">
-        <v>2</v>
-      </c>
-      <c r="H10" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="11">
       <c r="B11" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="C11" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="D11" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12">
@@ -335,33 +297,70 @@
         <v>0</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C12" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="D12" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="E12" t="s">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="F12" t="s">
-        <v>27</v>
+        <v>4</v>
       </c>
       <c r="G12" t="s">
-        <v>28</v>
+        <v>2</v>
+      </c>
+      <c r="H12" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="13">
       <c r="B13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" t="s">
+        <v>26</v>
+      </c>
+      <c r="F14" t="s">
+        <v>27</v>
+      </c>
+      <c r="G14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" t="s">
         <v>21</v>
       </c>
-      <c r="C13" t="n">
+      <c r="C15" t="n">
         <v>2.0</v>
       </c>
-      <c r="D13" t="s">
-        <v>29</v>
+      <c r="D15" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>